<commit_message>
More work on JPADCore_v2 concerning weights analysis.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
@@ -298,7 +298,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>825.0539956803455</v>
+        <v>3999.999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -336,7 +336,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>25070.404491806272</v>
+        <v>27512.318491806276</v>
       </c>
     </row>
     <row r="7">
@@ -347,7 +347,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>245856.68220957194</v>
+        <v>269803.6781376719</v>
       </c>
     </row>
     <row r="8">
@@ -358,7 +358,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>24690.447825139614</v>
+        <v>23673.118491806283</v>
       </c>
     </row>
     <row r="9">
@@ -369,7 +369,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>242130.58016440534</v>
+        <v>232153.98745767202</v>
       </c>
     </row>
     <row r="10">
@@ -380,7 +380,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>22577.803042625652</v>
+        <v>21662.206642625653</v>
       </c>
     </row>
     <row r="11">
@@ -391,7 +391,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="n">
-        <v>221412.6122079648</v>
+        <v>212433.67877190482</v>
       </c>
     </row>
     <row r="12">
@@ -468,7 +468,7 @@
         <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>20131.956045198745</v>
+        <v>19114.626711865414</v>
       </c>
     </row>
     <row r="19">
@@ -479,7 +479,7 @@
         <v>12</v>
       </c>
       <c r="C19" t="n">
-        <v>197427.04675064824</v>
+        <v>187450.4540439149</v>
       </c>
     </row>
     <row r="20">
@@ -490,7 +490,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="n">
-        <v>19735.956045198745</v>
+        <v>18718.626711865414</v>
       </c>
     </row>
     <row r="21">
@@ -501,7 +501,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="n">
-        <v>193543.61335064823</v>
+        <v>183567.02064391493</v>
       </c>
     </row>
     <row r="22">
@@ -512,7 +512,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="n">
-        <v>13003.956045198749</v>
+        <v>11986.626711865418</v>
       </c>
     </row>
     <row r="23">
@@ -523,7 +523,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>127525.24555064828</v>
+        <v>117548.65284391496</v>
       </c>
     </row>
     <row r="24">
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="n">
-        <v>12774.412399698747</v>
+        <v>10757.083066365416</v>
       </c>
     </row>
     <row r="25">
@@ -545,7 +545,7 @@
         <v>12</v>
       </c>
       <c r="C25" t="n">
-        <v>125274.19135950568</v>
+        <v>105490.94865277238</v>
       </c>
     </row>
     <row r="26">
@@ -556,7 +556,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="n">
-        <v>12188.456399698749</v>
+        <v>10739.123066365419</v>
       </c>
     </row>
     <row r="27">
@@ -567,7 +567,7 @@
         <v>12</v>
       </c>
       <c r="C27" t="n">
-        <v>119527.92595210572</v>
+        <v>105314.82121877241</v>
       </c>
     </row>
     <row r="28">
@@ -578,7 +578,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="n">
-        <v>585.9559999999999</v>
+        <v>1017.96</v>
       </c>
     </row>
     <row r="29">
@@ -589,7 +589,7 @@
         <v>12</v>
       </c>
       <c r="C29" t="n">
-        <v>5746.265407399998</v>
+        <v>9982.777433999996</v>
       </c>
     </row>
     <row r="30">
@@ -600,7 +600,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0</v>
+        <v>1000.0</v>
       </c>
     </row>
     <row r="31">
@@ -611,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0</v>
+        <v>9806.649999999998</v>
       </c>
     </row>
     <row r="32">
@@ -622,7 +622,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="n">
-        <v>13003.956045198749</v>
+        <v>11986.626711865418</v>
       </c>
     </row>
     <row r="33">
@@ -633,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="C33" t="n">
-        <v>127525.24555064828</v>
+        <v>117548.65284391496</v>
       </c>
     </row>
   </sheetData>
@@ -703,10 +703,10 @@
         <v>42</v>
       </c>
       <c r="C6" t="n">
-        <v>3484.0</v>
+        <v>1863.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4.2926420403520495</v>
+        <v>-44.23157516613781</v>
       </c>
     </row>
     <row r="7">
@@ -717,10 +717,10 @@
         <v>42</v>
       </c>
       <c r="C7" t="n">
-        <v>2460.0</v>
+        <v>1876.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-26.360534035801937</v>
+        <v>-43.84242351673351</v>
       </c>
     </row>
     <row r="8">
@@ -731,10 +731,10 @@
         <v>42</v>
       </c>
       <c r="C8" t="n">
-        <v>3024.0</v>
+        <v>3217.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-9.47733940010775</v>
+        <v>-3.6999341435670083</v>
       </c>
     </row>
     <row r="9">
@@ -745,10 +745,10 @@
         <v>42</v>
       </c>
       <c r="C9" t="n">
-        <v>2833.0</v>
+        <v>1987.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-15.194875172124753</v>
+        <v>-40.51966712566604</v>
       </c>
     </row>
     <row r="10">
@@ -787,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>2998.333333333333</v>
+        <v>1863.0</v>
       </c>
     </row>
   </sheetData>
@@ -825,7 +825,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>2006.3578899999998</v>
+        <v>22000.0</v>
       </c>
     </row>
     <row r="3">
@@ -868,10 +868,10 @@
         <v>42</v>
       </c>
       <c r="C7" t="n">
-        <v>2409.0</v>
+        <v>2454.0</v>
       </c>
       <c r="D7" t="n">
-        <v>20.068309448021772</v>
+        <v>-88.84545454545454</v>
       </c>
     </row>
     <row r="8">
@@ -882,10 +882,10 @@
         <v>42</v>
       </c>
       <c r="C8" t="n">
-        <v>1793.0</v>
+        <v>1921.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-10.634089314942699</v>
+        <v>-91.26818181818182</v>
       </c>
     </row>
     <row r="9">
@@ -896,10 +896,10 @@
         <v>42</v>
       </c>
       <c r="C9" t="n">
-        <v>2117.0</v>
+        <v>1641.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.514574969473679</v>
+        <v>-92.5409090909091</v>
       </c>
     </row>
     <row r="10">
@@ -913,7 +913,7 @@
         <v>2299.0</v>
       </c>
       <c r="D10" t="n">
-        <v>14.585738240349546</v>
+        <v>-89.55</v>
       </c>
     </row>
     <row r="11">
@@ -924,10 +924,10 @@
         <v>42</v>
       </c>
       <c r="C11" t="n">
-        <v>2493.0</v>
+        <v>2413.0</v>
       </c>
       <c r="D11" t="n">
-        <v>24.25500018842602</v>
+        <v>-89.03181818181818</v>
       </c>
     </row>
     <row r="12">
@@ -938,10 +938,10 @@
         <v>42</v>
       </c>
       <c r="C12" t="n">
-        <v>2235.0</v>
+        <v>2271.0</v>
       </c>
       <c r="D12" t="n">
-        <v>11.395878628612978</v>
+        <v>-89.67727272727272</v>
       </c>
     </row>
     <row r="13">
@@ -952,7 +952,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>2110.9999999999995</v>
+        <v>1641.0</v>
       </c>
     </row>
   </sheetData>
@@ -990,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>300.95368349999995</v>
+        <v>3299.9999999999995</v>
       </c>
     </row>
     <row r="3">
@@ -1036,7 +1036,7 @@
         <v>258.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-14.272522934579703</v>
+        <v>-92.18181818181817</v>
       </c>
     </row>
     <row r="8">
@@ -1047,10 +1047,10 @@
         <v>42</v>
       </c>
       <c r="C8" t="n">
-        <v>149.0</v>
+        <v>150.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-50.49072060950533</v>
+        <v>-95.45454545454544</v>
       </c>
     </row>
     <row r="9">
@@ -1061,10 +1061,10 @@
         <v>42</v>
       </c>
       <c r="C9" t="n">
-        <v>133.0</v>
+        <v>144.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-55.807153295732945</v>
+        <v>-95.63636363636363</v>
       </c>
     </row>
     <row r="10">
@@ -1075,7 +1075,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>257.99999999999994</v>
+        <v>258.0</v>
       </c>
     </row>
   </sheetData>
@@ -1113,7 +1113,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>300.95368349999995</v>
+        <v>3299.9999999999995</v>
       </c>
     </row>
     <row r="3">
@@ -1159,7 +1159,7 @@
         <v>330.0</v>
       </c>
       <c r="D7" t="n">
-        <v>9.651424153444566</v>
+        <v>-89.99999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -1170,10 +1170,10 @@
         <v>42</v>
       </c>
       <c r="C8" t="n">
-        <v>228.0</v>
+        <v>232.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-24.24083422125648</v>
+        <v>-92.96969696969695</v>
       </c>
     </row>
     <row r="9">
@@ -1184,7 +1184,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>329.99999999999994</v>
+        <v>330.0</v>
       </c>
     </row>
   </sheetData>
@@ -1233,10 +1233,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>645.9999999999998</v>
+        <v>712.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-21.10405471421592</v>
+        <v>-13.043478260869545</v>
       </c>
     </row>
     <row r="4">
@@ -1292,10 +1292,10 @@
         <v>42</v>
       </c>
       <c r="C10" t="n">
-        <v>540.0</v>
+        <v>356.0</v>
       </c>
       <c r="D10" t="n">
-        <v>31.90034196384954</v>
+        <v>-13.043478260869561</v>
       </c>
     </row>
     <row r="11">
@@ -1320,7 +1320,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>323.0</v>
+        <v>356.0</v>
       </c>
     </row>
     <row r="13">
@@ -1366,10 +1366,10 @@
         <v>42</v>
       </c>
       <c r="C17" t="n">
-        <v>540.0</v>
+        <v>356.0</v>
       </c>
       <c r="D17" t="n">
-        <v>31.90034196384954</v>
+        <v>-13.043478260869561</v>
       </c>
     </row>
     <row r="18">
@@ -1394,7 +1394,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>323.0</v>
+        <v>356.0</v>
       </c>
     </row>
     <row r="20">
@@ -1451,7 +1451,7 @@
         <v>1447.8668450399996</v>
       </c>
       <c r="D3" t="n">
-        <v>-21.10405471421592</v>
+        <v>-13.043478260869545</v>
       </c>
     </row>
     <row r="4">
@@ -1579,7 +1579,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>987.8878901438338</v>
+        <v>1057.4352685771673</v>
       </c>
     </row>
     <row r="4">
@@ -1600,10 +1600,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>821.0</v>
+        <v>911.0</v>
       </c>
       <c r="D6" t="n">
-        <v>21.48564664101806</v>
+        <v>34.80319621189702</v>
       </c>
     </row>
     <row r="7">
@@ -1614,10 +1614,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>1003.0</v>
+        <v>1135.0</v>
       </c>
       <c r="D7" t="n">
-        <v>48.41669132879551</v>
+        <v>67.94909736608466</v>
       </c>
     </row>
     <row r="8">
@@ -1628,10 +1628,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>1135.0</v>
+        <v>1281.0</v>
       </c>
       <c r="D8" t="n">
-        <v>67.94909736608466</v>
+        <v>89.55312222551052</v>
       </c>
     </row>
     <row r="9">
@@ -1642,10 +1642,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>988.0</v>
+        <v>1057.0</v>
       </c>
       <c r="D9" t="n">
-        <v>46.19709973364902</v>
+        <v>56.407221071322894</v>
       </c>
     </row>
     <row r="10">
@@ -1656,7 +1656,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>821.0</v>
+        <v>911.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on the weights estimation and engines.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Maximum Passengers Mass</t>
+  </si>
+  <si>
+    <t>Maximum Fuel Mass</t>
   </si>
   <si>
     <t>Fuel Mass</t>
@@ -301,7 +304,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>200.0</v>
+        <v>1200.0</v>
       </c>
     </row>
     <row r="3">
@@ -323,7 +326,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>99.0</v>
+        <v>93.0</v>
       </c>
     </row>
     <row r="5">
@@ -339,7 +342,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>24956.015437694587</v>
+        <v>26046.215258116197</v>
       </c>
     </row>
     <row r="7">
@@ -350,7 +353,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>24560.015437694587</v>
+        <v>25674.215258116197</v>
       </c>
     </row>
     <row r="8">
@@ -361,7 +364,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>22460.413893925128</v>
+        <v>25264.828800372707</v>
       </c>
     </row>
     <row r="9">
@@ -372,7 +375,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>7128.0</v>
+        <v>6696.0</v>
       </c>
     </row>
     <row r="10">
@@ -394,7 +397,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>229.54364550000003</v>
+        <v>6889.111532305973</v>
       </c>
     </row>
     <row r="12">
@@ -405,7 +408,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>20001.523657753718</v>
+        <v>229.54364550000003</v>
       </c>
     </row>
     <row r="13">
@@ -416,7 +419,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>19605.523657753718</v>
+        <v>19157.103725810226</v>
       </c>
     </row>
     <row r="14">
@@ -427,7 +430,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>12873.523657753718</v>
+        <v>18785.103725810226</v>
       </c>
     </row>
     <row r="15">
@@ -438,7 +441,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>11643.980012253716</v>
+        <v>12461.10372581023</v>
       </c>
     </row>
     <row r="16">
@@ -449,7 +452,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>12058.024012253722</v>
+        <v>12231.560080310228</v>
       </c>
     </row>
     <row r="17">
@@ -460,7 +463,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>585.9559999999999</v>
+        <v>11611.13608031023</v>
       </c>
     </row>
     <row r="18">
@@ -471,34 +474,34 @@
         <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>1000.0</v>
+        <v>620.424</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="n">
-        <v>244734.90879206755</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
       <c r="C21" t="n">
-        <v>240851.47539206757</v>
+        <v>255426.11686100514</v>
       </c>
     </row>
     <row r="22">
@@ -506,10 +509,10 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" t="n">
-        <v>220261.4179128608</v>
+        <v>251778.04306100513</v>
       </c>
     </row>
     <row r="23">
@@ -517,10 +520,10 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" t="n">
-        <v>69901.80119999999</v>
+        <v>247763.33335517492</v>
       </c>
     </row>
     <row r="24">
@@ -528,10 +531,10 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" t="n">
-        <v>48586.96681375712</v>
+        <v>65665.32839999997</v>
       </c>
     </row>
     <row r="25">
@@ -539,10 +542,10 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" t="n">
-        <v>2251.0541911425744</v>
+        <v>48586.96681375712</v>
       </c>
     </row>
     <row r="26">
@@ -550,10 +553,10 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>196147.94197831047</v>
+        <v>2251.0541911425744</v>
       </c>
     </row>
     <row r="27">
@@ -561,10 +564,10 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>192264.50857831046</v>
+        <v>187867.01125271677</v>
       </c>
     </row>
     <row r="28">
@@ -572,10 +575,10 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C28" t="n">
-        <v>126246.14077831048</v>
+        <v>184218.9374527168</v>
       </c>
     </row>
     <row r="29">
@@ -583,10 +586,10 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C29" t="n">
-        <v>114188.43658716789</v>
+        <v>122201.68285271685</v>
       </c>
     </row>
     <row r="30">
@@ -594,10 +597,10 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C30" t="n">
-        <v>118248.82117976793</v>
+        <v>119950.62866157427</v>
       </c>
     </row>
     <row r="31">
@@ -605,10 +608,10 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C31" t="n">
-        <v>5746.265407399998</v>
+        <v>113866.3476419743</v>
       </c>
     </row>
     <row r="32">
@@ -616,10 +619,21 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C32" t="n">
-        <v>9806.649999999998</v>
+        <v>6084.281019599997</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -646,23 +660,23 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>3000.0</v>
+        <v>2509.087499999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -678,105 +692,105 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" t="n">
-        <v>3234.0</v>
+        <v>3661.0</v>
       </c>
       <c r="D6" t="n">
-        <v>7.8</v>
+        <v>45.90961853661946</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="n">
-        <v>2371.0</v>
+        <v>2549.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-20.966666666666665</v>
+        <v>1.590717741011475</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>3023.0</v>
+        <v>3077.0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7666666666666667</v>
+        <v>22.63422459360232</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>2676.0</v>
+        <v>3038.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-10.8</v>
+        <v>21.07987465562686</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" t="n">
         <v>2491.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-16.966666666666665</v>
+        <v>-0.7208796026443373</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="n">
         <v>3698.0</v>
       </c>
       <c r="D11" t="n">
-        <v>23.266666666666666</v>
+        <v>47.384258221365414</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>2915.5</v>
+        <v>3085.666666666666</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.816666666666666</v>
+        <v>22.979635690930156</v>
       </c>
     </row>
   </sheetData>
@@ -803,23 +817,23 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>2000.0</v>
+        <v>1672.7249999999997</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -830,7 +844,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -846,105 +860,105 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="n">
-        <v>2407.0</v>
+        <v>2400.0</v>
       </c>
       <c r="D7" t="n">
-        <v>20.35</v>
+        <v>43.47845581311936</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>1792.0</v>
+        <v>1680.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-10.4</v>
+        <v>0.43491906918355067</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>2027.0</v>
+        <v>1964.0</v>
       </c>
       <c r="D9" t="n">
-        <v>1.35</v>
+        <v>17.41320300706934</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" t="n">
-        <v>2298.0</v>
+        <v>2299.0</v>
       </c>
       <c r="D10" t="n">
-        <v>14.9</v>
+        <v>37.44040413098392</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="n">
-        <v>2489.0</v>
+        <v>2669.0</v>
       </c>
       <c r="D11" t="n">
-        <v>24.45</v>
+        <v>59.559999402173155</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="n">
-        <v>2233.0</v>
+        <v>2222.0</v>
       </c>
       <c r="D12" t="n">
-        <v>11.65</v>
+        <v>32.837137006979674</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>1892.2857142857142</v>
+        <v>1890.5714285714284</v>
       </c>
       <c r="D13" t="n">
-        <v>-5.385714285714288</v>
+        <v>13.023445489929836</v>
       </c>
     </row>
   </sheetData>
@@ -971,23 +985,23 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>600.0</v>
+        <v>250.90874999999994</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -998,7 +1012,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1014,63 +1028,63 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="n">
         <v>258.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-57.0</v>
+        <v>2.826226666068864</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="n">
         <v>149.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-75.16666666666667</v>
+        <v>-40.6158613440145</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>133.0</v>
+        <v>136.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-77.83333333333333</v>
+        <v>-45.79702780393269</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>180.0</v>
+        <v>181.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-69.99999999999999</v>
+        <v>-27.862220827292767</v>
       </c>
     </row>
   </sheetData>
@@ -1097,23 +1111,23 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>400.0</v>
+        <v>250.90874999999994</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1124,7 +1138,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1140,49 +1154,49 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="n">
         <v>330.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-17.5</v>
+        <v>31.521917828692732</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>228.0</v>
+        <v>225.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-43.0</v>
+        <v>-10.32596511680041</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>279.0</v>
+        <v>277.5</v>
       </c>
       <c r="D9" t="n">
-        <v>-30.25</v>
+        <v>10.597976355946154</v>
       </c>
     </row>
   </sheetData>
@@ -1209,32 +1223,32 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>900.0</v>
+        <v>250.90874999999994</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>628.6666666666665</v>
+        <v>243.99999999999994</v>
       </c>
       <c r="D3" t="n">
-        <v>-76.71604938271604</v>
+        <v>-67.58449701999895</v>
       </c>
     </row>
     <row r="4">
@@ -1244,7 +1258,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
@@ -1254,12 +1268,12 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1268,55 +1282,55 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>235.0</v>
+        <v>52.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-47.777777777777764</v>
+        <v>-58.5506683206544</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" t="n">
-        <v>514.0</v>
+        <v>558.0</v>
       </c>
       <c r="D10" t="n">
-        <v>14.22222222222225</v>
+        <v>344.7832130206701</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="n">
-        <v>194.0</v>
+        <v>192.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-56.88888888888888</v>
+        <v>53.043686200660666</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>314.33333333333326</v>
+        <v>122.0</v>
       </c>
     </row>
     <row r="13">
@@ -1326,12 +1340,12 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1340,55 +1354,55 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" t="n">
-        <v>235.0</v>
+        <v>52.0</v>
       </c>
       <c r="D16" t="n">
-        <v>-47.777777777777764</v>
+        <v>-58.5506683206544</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" t="n">
-        <v>514.0</v>
+        <v>558.0</v>
       </c>
       <c r="D17" t="n">
-        <v>14.22222222222225</v>
+        <v>344.7832130206701</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" t="n">
-        <v>194.0</v>
+        <v>192.0</v>
       </c>
       <c r="D18" t="n">
-        <v>-56.88888888888888</v>
+        <v>53.043686200660666</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>314.33333333333326</v>
+        <v>122.0</v>
       </c>
     </row>
     <row r="20">
@@ -1422,7 +1436,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1433,13 +1447,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>1447.8668450399996</v>
+        <v>1329.141763746719</v>
       </c>
     </row>
     <row r="4">
@@ -1449,7 +1463,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
@@ -1459,12 +1473,12 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1475,13 +1489,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>723.9334225199998</v>
+        <v>664.5708818733597</v>
       </c>
     </row>
     <row r="10">
@@ -1491,12 +1505,12 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1507,13 +1521,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>723.9334225199998</v>
+        <v>664.5708818733597</v>
       </c>
     </row>
     <row r="14">
@@ -1545,18 +1559,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>500.0</v>
+        <v>669.0899999999998</v>
       </c>
     </row>
     <row r="3">
@@ -1566,77 +1580,77 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>820.0</v>
+        <v>845.0</v>
       </c>
       <c r="D5" t="n">
-        <v>64.0</v>
+        <v>26.290932460506117</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>1002.0</v>
+        <v>1038.0</v>
       </c>
       <c r="D6" t="n">
-        <v>100.4</v>
+        <v>55.13608034793533</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>1134.0</v>
+        <v>1174.0</v>
       </c>
       <c r="D7" t="n">
-        <v>126.8</v>
+        <v>75.46219492146056</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>987.0</v>
+        <v>1051.0</v>
       </c>
       <c r="D8" t="n">
-        <v>97.4</v>
+        <v>57.07901777040465</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>985.75</v>
+        <v>1027.0</v>
       </c>
       <c r="D9" t="n">
-        <v>97.14999999999998</v>
+        <v>53.492056375076615</v>
       </c>
     </row>
   </sheetData>
@@ -1663,18 +1677,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>2000.0</v>
+        <v>669.0899999999998</v>
       </c>
     </row>
     <row r="3">
@@ -1684,35 +1698,35 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>2477.0</v>
+        <v>2324.0</v>
       </c>
       <c r="D5" t="n">
-        <v>23.85</v>
+        <v>247.33742844759317</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>2476.9547862613454</v>
+        <v>2324.2562213254223</v>
       </c>
       <c r="D6" t="n">
-        <v>23.84773931306728</v>
+        <v>247.37572244771587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on databae serializaition.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
@@ -308,7 +308,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>1375.293247</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="3">
@@ -330,7 +330,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>106.0</v>
+        <v>95.0</v>
       </c>
     </row>
     <row r="5">
@@ -346,7 +346,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>27020.304767035734</v>
+        <v>21956.0753832672</v>
       </c>
     </row>
     <row r="7">
@@ -357,7 +357,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>26596.304767035734</v>
+        <v>21576.0753832672</v>
       </c>
     </row>
     <row r="8">
@@ -368,7 +368,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>26209.695624024658</v>
+        <v>21297.393121769186</v>
       </c>
     </row>
     <row r="9">
@@ -379,7 +379,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>7632.0</v>
+        <v>6840.0</v>
       </c>
     </row>
     <row r="10">
@@ -401,7 +401,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>5708.403422177888</v>
+        <v>3036.328800314118</v>
       </c>
     </row>
     <row r="12">
@@ -423,7 +423,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>21311.901344857844</v>
+        <v>18919.746582953085</v>
       </c>
     </row>
     <row r="14">
@@ -434,7 +434,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>20887.901344857844</v>
+        <v>18539.746582953085</v>
       </c>
     </row>
     <row r="15">
@@ -445,7 +445,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>13679.901344857848</v>
+        <v>12079.746582953088</v>
       </c>
     </row>
     <row r="16">
@@ -456,7 +456,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>13450.357699357846</v>
+        <v>11850.202937453087</v>
       </c>
     </row>
     <row r="17">
@@ -467,7 +467,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>12829.93369935785</v>
+        <v>11229.778937453088</v>
       </c>
     </row>
     <row r="18">
@@ -505,7 +505,7 @@
         <v>25</v>
       </c>
       <c r="C21" t="n">
-        <v>264978.6717436509</v>
+        <v>215315.54665731726</v>
       </c>
     </row>
     <row r="22">
@@ -516,7 +516,7 @@
         <v>25</v>
       </c>
       <c r="C22" t="n">
-        <v>260820.65214365092</v>
+        <v>211589.01965731726</v>
       </c>
     </row>
     <row r="23">
@@ -527,7 +527,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="n">
-        <v>257029.31159134133</v>
+        <v>208856.08025759773</v>
       </c>
     </row>
     <row r="24">
@@ -538,7 +538,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="n">
-        <v>74844.35279999998</v>
+        <v>67077.48599999998</v>
       </c>
     </row>
     <row r="25">
@@ -571,7 +571,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>208998.3573235501</v>
+        <v>185539.33282771683</v>
       </c>
     </row>
     <row r="28">
@@ -582,7 +582,7 @@
         <v>25</v>
       </c>
       <c r="C28" t="n">
-        <v>204840.3377235501</v>
+        <v>181812.80582771683</v>
       </c>
     </row>
     <row r="29">
@@ -593,7 +593,7 @@
         <v>25</v>
       </c>
       <c r="C29" t="n">
-        <v>134154.00452355016</v>
+        <v>118461.84682771686</v>
       </c>
     </row>
     <row r="30">
@@ -604,7 +604,7 @@
         <v>25</v>
       </c>
       <c r="C30" t="n">
-        <v>131902.95033240755</v>
+        <v>116210.79263657428</v>
       </c>
     </row>
     <row r="31">
@@ -615,7 +615,7 @@
         <v>25</v>
       </c>
       <c r="C31" t="n">
-        <v>125818.66931280764</v>
+        <v>110126.51161697431</v>
       </c>
     </row>
     <row r="32">
@@ -679,7 +679,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>6031.124999999998</v>
+        <v>2606.624999999999</v>
       </c>
     </row>
     <row r="3">
@@ -714,7 +714,7 @@
         <v>3372.0</v>
       </c>
       <c r="D6" t="n">
-        <v>-44.09003295405085</v>
+        <v>29.3626816285427</v>
       </c>
     </row>
     <row r="7">
@@ -725,10 +725,10 @@
         <v>43</v>
       </c>
       <c r="C7" t="n">
-        <v>2478.0</v>
+        <v>2322.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-58.91313809612633</v>
+        <v>-10.919292188174332</v>
       </c>
     </row>
     <row r="8">
@@ -739,10 +739,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>3140.0</v>
+        <v>2830.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-47.93674480300108</v>
+        <v>8.569510382199242</v>
       </c>
     </row>
     <row r="9">
@@ -753,10 +753,10 @@
         <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>2968.0</v>
+        <v>2437.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-50.78861738067109</v>
+        <v>-6.507456960629133</v>
       </c>
     </row>
     <row r="10">
@@ -770,7 +770,7 @@
         <v>2491.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-58.69758958734895</v>
+        <v>-4.435812592912257</v>
       </c>
     </row>
     <row r="11">
@@ -784,7 +784,7 @@
         <v>3698.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-38.684739580094906</v>
+        <v>41.86927540401865</v>
       </c>
     </row>
     <row r="12">
@@ -795,10 +795,10 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>3024.5</v>
+        <v>2858.333333333333</v>
       </c>
       <c r="D12" t="n">
-        <v>-49.85181040021553</v>
+        <v>9.656484278840807</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +840,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>4020.749999999999</v>
+        <v>1737.7499999999995</v>
       </c>
     </row>
     <row r="3">
@@ -883,10 +883,10 @@
         <v>43</v>
       </c>
       <c r="C7" t="n">
-        <v>2488.0</v>
+        <v>2302.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-38.12099732636945</v>
+        <v>32.470148180118</v>
       </c>
     </row>
     <row r="8">
@@ -897,10 +897,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>2738.0</v>
+        <v>1716.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-31.903251880867984</v>
+        <v>-1.251618472162253</v>
       </c>
     </row>
     <row r="9">
@@ -911,10 +911,10 @@
         <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>3913.0</v>
+        <v>1934.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.6798482870111076</v>
+        <v>11.29333908790105</v>
       </c>
     </row>
     <row r="10">
@@ -928,7 +928,7 @@
         <v>2299.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-42.82161288316855</v>
+        <v>32.29751114947493</v>
       </c>
     </row>
     <row r="11">
@@ -939,10 +939,10 @@
         <v>43</v>
       </c>
       <c r="C11" t="n">
-        <v>4931.0</v>
+        <v>2741.0</v>
       </c>
       <c r="D11" t="n">
-        <v>22.63881116707085</v>
+        <v>57.73270033088768</v>
       </c>
     </row>
     <row r="12">
@@ -953,10 +953,10 @@
         <v>43</v>
       </c>
       <c r="C12" t="n">
-        <v>3506.0</v>
+        <v>2257.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-12.80233787228749</v>
+        <v>29.880592720471906</v>
       </c>
     </row>
     <row r="13">
@@ -967,10 +967,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>2839.2857142857138</v>
+        <v>1892.7142857142858</v>
       </c>
       <c r="D13" t="n">
-        <v>-29.384176726090526</v>
+        <v>8.917524713813041</v>
       </c>
     </row>
   </sheetData>
@@ -1012,7 +1012,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>603.1124999999997</v>
+        <v>260.6624999999999</v>
       </c>
     </row>
     <row r="3">
@@ -1058,7 +1058,7 @@
         <v>258.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-57.22191133494992</v>
+        <v>-1.0214357646381471</v>
       </c>
     </row>
     <row r="8">
@@ -1072,7 +1072,7 @@
         <v>149.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-75.29482476320752</v>
+        <v>-42.83796096484916</v>
       </c>
     </row>
     <row r="9">
@@ -1083,10 +1083,10 @@
         <v>43</v>
       </c>
       <c r="C9" t="n">
-        <v>140.0</v>
+        <v>122.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-76.78708367012787</v>
+        <v>-53.196182803433544</v>
       </c>
     </row>
     <row r="10">
@@ -1097,10 +1097,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>182.33333333333331</v>
+        <v>176.33333333333331</v>
       </c>
       <c r="D10" t="n">
-        <v>-69.76793992276176</v>
+        <v>-32.351859844306944</v>
       </c>
     </row>
   </sheetData>
@@ -1142,7 +1142,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>603.1124999999997</v>
+        <v>260.6624999999999</v>
       </c>
     </row>
     <row r="3">
@@ -1188,7 +1188,7 @@
         <v>330.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-45.283840079587115</v>
+        <v>26.600489138253533</v>
       </c>
     </row>
     <row r="8">
@@ -1199,10 +1199,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="n">
-        <v>262.0</v>
+        <v>226.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-56.55868515409644</v>
+        <v>-13.297846832590004</v>
       </c>
     </row>
     <row r="9">
@@ -1213,10 +1213,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>296.0</v>
+        <v>278.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-50.92126261684178</v>
+        <v>6.651321152831752</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1258,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>603.1124999999997</v>
+        <v>260.6624999999999</v>
       </c>
     </row>
     <row r="3">
@@ -1269,10 +1269,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>514.6666666666665</v>
+        <v>243.99999999999994</v>
       </c>
       <c r="D3" t="n">
-        <v>-71.55496602117255</v>
+        <v>-68.79745520228902</v>
       </c>
     </row>
     <row r="4">
@@ -1315,7 +1315,7 @@
         <v>52.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-82.75611929780926</v>
+        <v>-60.10166402915646</v>
       </c>
     </row>
     <row r="10">
@@ -1329,7 +1329,7 @@
         <v>528.0</v>
       </c>
       <c r="D10" t="n">
-        <v>75.09171174532123</v>
+        <v>305.12156524241135</v>
       </c>
     </row>
     <row r="11">
@@ -1343,7 +1343,7 @@
         <v>192.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-36.330286638065004</v>
+        <v>47.31693281542229</v>
       </c>
     </row>
     <row r="12">
@@ -1354,7 +1354,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>257.33333333333326</v>
+        <v>122.0</v>
       </c>
     </row>
     <row r="13">
@@ -1387,7 +1387,7 @@
         <v>52.0</v>
       </c>
       <c r="D16" t="n">
-        <v>-82.75611929780926</v>
+        <v>-60.10166402915646</v>
       </c>
     </row>
     <row r="17">
@@ -1401,7 +1401,7 @@
         <v>528.0</v>
       </c>
       <c r="D17" t="n">
-        <v>75.09171174532123</v>
+        <v>305.12156524241135</v>
       </c>
     </row>
     <row r="18">
@@ -1415,7 +1415,7 @@
         <v>192.0</v>
       </c>
       <c r="D18" t="n">
-        <v>-36.330286638065004</v>
+        <v>47.31693281542229</v>
       </c>
     </row>
     <row r="19">
@@ -1426,7 +1426,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>257.33333333333326</v>
+        <v>122.0</v>
       </c>
     </row>
     <row r="20">
@@ -1602,7 +1602,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>1608.2999999999997</v>
+        <v>695.0999999999998</v>
       </c>
     </row>
     <row r="3">
@@ -1623,10 +1623,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>874.0</v>
+        <v>734.0</v>
       </c>
       <c r="D5" t="n">
-        <v>-45.65690480631722</v>
+        <v>5.596317076679663</v>
       </c>
     </row>
     <row r="6">
@@ -1637,10 +1637,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>1081.0</v>
+        <v>878.0</v>
       </c>
       <c r="D6" t="n">
-        <v>-32.78617173412919</v>
+        <v>26.312760753848426</v>
       </c>
     </row>
     <row r="7">
@@ -1651,10 +1651,10 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>1221.0</v>
+        <v>998.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-24.081328110427144</v>
+        <v>43.57646381815573</v>
       </c>
     </row>
     <row r="8">
@@ -1665,10 +1665,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>1095.0</v>
+        <v>890.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-31.915687371758988</v>
+        <v>28.039131060279157</v>
       </c>
     </row>
     <row r="9">
@@ -1679,10 +1679,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>1067.75</v>
+        <v>875.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-33.61002300565813</v>
+        <v>25.88116817724071</v>
       </c>
     </row>
   </sheetData>
@@ -1724,7 +1724,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>1608.2999999999997</v>
+        <v>695.0999999999998</v>
       </c>
     </row>
     <row r="3">
@@ -1748,7 +1748,7 @@
         <v>2324.0</v>
       </c>
       <c r="D5" t="n">
-        <v>44.500404153453985</v>
+        <v>234.3403826787514</v>
       </c>
     </row>
     <row r="6">
@@ -1762,7 +1762,7 @@
         <v>2324.2562213254223</v>
       </c>
       <c r="D6" t="n">
-        <v>44.516335343245814</v>
+        <v>234.37724375275826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on ACPerformanceManager. More tests.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="70">
   <si>
     <t>Description</t>
   </si>
@@ -115,25 +115,25 @@
     <t>WEIGHT ESTIMATION METHODS COMPARISON</t>
   </si>
   <si>
+    <t>TORENBEEK_1976</t>
+  </si>
+  <si>
     <t>RAYMER</t>
   </si>
   <si>
     <t>KROO</t>
   </si>
   <si>
-    <t>TORENBEEK_1976</t>
+    <t>SADRAEY</t>
+  </si>
+  <si>
+    <t>NICOLAI_1984</t>
+  </si>
+  <si>
+    <t>JENKINSON</t>
   </si>
   <si>
     <t>TORENBEEK_2013</t>
-  </si>
-  <si>
-    <t>NICOLAI_1984</t>
-  </si>
-  <si>
-    <t>JENKINSON</t>
-  </si>
-  <si>
-    <t>SADRAEY</t>
   </si>
   <si>
     <t>ROSKAM</t>
@@ -347,7 +347,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>25039.059859733283</v>
+        <v>27207.06814830184</v>
       </c>
     </row>
     <row r="6">
@@ -358,7 +358,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>24631.059859733283</v>
+        <v>26799.06814830184</v>
       </c>
     </row>
     <row r="7">
@@ -369,7 +369,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>24287.888063941282</v>
+        <v>24486.361333471657</v>
       </c>
     </row>
     <row r="8">
@@ -380,7 +380,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>4954.49177994087</v>
+        <v>5149.210094359609</v>
       </c>
     </row>
     <row r="9">
@@ -391,7 +391,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>4836.916567029353</v>
+        <v>5255.574895193706</v>
       </c>
     </row>
     <row r="10">
@@ -402,7 +402,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>20202.14329270393</v>
+        <v>21951.493253108136</v>
       </c>
     </row>
     <row r="11">
@@ -413,7 +413,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>19794.14329270393</v>
+        <v>21543.493253108136</v>
       </c>
     </row>
     <row r="12">
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>12858.143292703935</v>
+        <v>14607.493253108136</v>
       </c>
     </row>
     <row r="15">
@@ -457,7 +457,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>12628.599647203933</v>
+        <v>14377.949607608134</v>
       </c>
     </row>
     <row r="16">
@@ -501,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>12008.175647203934</v>
+        <v>13757.525607608139</v>
       </c>
     </row>
     <row r="20">
@@ -512,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>6340.505823186282</v>
+        <v>7941.499490393542</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2503.777472995741</v>
+        <v>2720.4914221436675</v>
       </c>
     </row>
     <row r="3">
@@ -565,10 +565,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>2926.875</v>
+        <v>3523.0</v>
       </c>
       <c r="D3" t="n">
-        <v>16.898367828912026</v>
+        <v>29.498662312413344</v>
       </c>
     </row>
     <row r="4">
@@ -590,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>2926.8749999999995</v>
+        <v>3522.9999999999995</v>
       </c>
     </row>
     <row r="6">
@@ -611,10 +611,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>3022.0</v>
+        <v>4094.0</v>
       </c>
       <c r="D8" t="n">
-        <v>20.69762718905733</v>
+        <v>50.48751731678124</v>
       </c>
     </row>
     <row r="9">
@@ -625,10 +625,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>2304.0</v>
+        <v>3151.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-7.979042672538686</v>
+        <v>15.824662204488938</v>
       </c>
     </row>
     <row r="10">
@@ -639,10 +639,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>3125.0</v>
+        <v>2378.0</v>
       </c>
       <c r="D10" t="n">
-        <v>24.81141130569297</v>
+        <v>-12.58932189074113</v>
       </c>
     </row>
     <row r="11">
@@ -653,10 +653,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>3698.0</v>
+        <v>2491.0</v>
       </c>
       <c r="D11" t="n">
-        <v>47.69683168270483</v>
+        <v>-8.435660567635056</v>
       </c>
     </row>
     <row r="12">
@@ -667,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>2503.0</v>
+        <v>3127.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.031052000592157212</v>
+        <v>14.942468649138975</v>
       </c>
     </row>
     <row r="13">
@@ -681,10 +681,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>3366.0</v>
+        <v>5004.0</v>
       </c>
       <c r="D13" t="n">
-        <v>34.43686734558801</v>
+        <v>83.93735629046735</v>
       </c>
     </row>
     <row r="14">
@@ -695,10 +695,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>2491.0</v>
+        <v>3698.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.5103278200060182</v>
+        <v>35.93132365350685</v>
       </c>
     </row>
     <row r="15">
@@ -709,10 +709,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>2906.0</v>
+        <v>4241.0</v>
       </c>
       <c r="D15" t="n">
-        <v>16.064627601390008</v>
+        <v>55.890952843299765</v>
       </c>
     </row>
   </sheetData>
@@ -754,7 +754,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2654.0041213754853</v>
+        <v>2883.7209074722878</v>
       </c>
     </row>
     <row r="3">
@@ -765,10 +765,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1870.1428571428569</v>
+        <v>2303.75</v>
       </c>
       <c r="D3" t="n">
-        <v>-29.535043217128766</v>
+        <v>-20.11189453075952</v>
       </c>
     </row>
     <row r="4">
@@ -790,7 +790,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>1870.1428571428569</v>
+        <v>2303.7499999999995</v>
       </c>
     </row>
     <row r="6">
@@ -805,16 +805,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>2551.0</v>
+        <v>2283.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-3.8810837008836714</v>
+        <v>-20.831450988051646</v>
       </c>
     </row>
     <row r="9">
@@ -825,10 +825,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>2411.0</v>
+        <v>2500.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-9.156132027765791</v>
+        <v>-13.306450928659272</v>
       </c>
     </row>
     <row r="10">
@@ -839,66 +839,24 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>2364.0</v>
+        <v>2308.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-10.92704110893336</v>
+        <v>-19.96451549733824</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2229.0</v>
+        <v>2124.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-16.013694852712547</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-100.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2463.0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-7.196828363495289</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1073.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-59.57052246611062</v>
+        <v>-26.345160708988917</v>
       </c>
     </row>
   </sheetData>
@@ -940,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>287.93440939451017</v>
+        <v>312.8565135465218</v>
       </c>
     </row>
     <row r="3">
@@ -951,10 +909,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>200.71428571428572</v>
+        <v>237.5</v>
       </c>
       <c r="D3" t="n">
-        <v>-30.29166394653469</v>
+        <v>-24.086605291443377</v>
       </c>
     </row>
     <row r="4">
@@ -976,7 +934,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>200.7142857142857</v>
+        <v>237.49999999999997</v>
       </c>
     </row>
     <row r="6">
@@ -997,10 +955,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>137.0</v>
+        <v>276.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-52.41971937702972</v>
+        <v>-11.780644465003677</v>
       </c>
     </row>
     <row r="9">
@@ -1011,80 +969,94 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>303.0</v>
+        <v>144.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5.232299479999953</v>
+        <v>-53.972510155654085</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>117.0</v>
+        <v>303.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-59.36574574534655</v>
+        <v>-3.1504901191888184</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>293.0</v>
+        <v>124.0</v>
       </c>
       <c r="D11" t="n">
-        <v>1.7592862958415385</v>
+        <v>-60.36521707847991</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>273.0</v>
+        <v>271.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-5.18674007247529</v>
+        <v>-13.378821195710133</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>141.0</v>
+        <v>293.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-51.03051410336636</v>
+        <v>-6.346843580601728</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>238.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-23.926787618372735</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>141.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-51.03051410336636</v>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="n">
+        <v>251.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-19.771528118535954</v>
       </c>
     </row>
   </sheetData>
@@ -1126,7 +1098,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>287.93440939451017</v>
+        <v>312.8565135465218</v>
       </c>
     </row>
     <row r="3">
@@ -1137,10 +1109,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>256.0</v>
+        <v>325.1428571428571</v>
       </c>
       <c r="D3" t="n">
-        <v>-11.090862485544614</v>
+        <v>3.9271496882254904</v>
       </c>
     </row>
     <row r="4">
@@ -1162,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>255.99999999999997</v>
+        <v>325.1428571428571</v>
       </c>
     </row>
     <row r="6">
@@ -1183,10 +1155,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>84.0</v>
+        <v>391.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-70.82668925306932</v>
+        <v>24.97742034124479</v>
       </c>
     </row>
     <row r="9">
@@ -1197,66 +1169,80 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>252.0</v>
+        <v>89.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-12.48006775920796</v>
+        <v>-71.55245419342509</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>330.0</v>
+        <v>257.0</v>
       </c>
       <c r="D10" t="n">
-        <v>14.60943507722767</v>
+        <v>-17.85371604168821</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>412.0</v>
+        <v>419.0</v>
       </c>
       <c r="D11" t="n">
-        <v>43.08814318732667</v>
+        <v>33.92721003320094</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>302.0</v>
+        <v>330.0</v>
       </c>
       <c r="D12" t="n">
-        <v>4.884998161584111</v>
+        <v>5.479664226626039</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>512.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>63.65329722434101</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>156.0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-45.82099432712874</v>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>278.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-11.141373772721094</v>
       </c>
     </row>
   </sheetData>
@@ -1298,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>475.7177198691908</v>
+        <v>516.8933702072968</v>
       </c>
     </row>
     <row r="3">
@@ -1312,7 +1298,7 @@
         <v>354.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-25.586122775216314</v>
+        <v>-31.513921360989688</v>
       </c>
     </row>
     <row r="4">
@@ -1359,30 +1345,30 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>179.0</v>
+        <v>175.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-24.745288004314787</v>
+        <v>-32.287775356910714</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>175.0</v>
+        <v>179.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-26.42695754611781</v>
+        <v>-30.740067365068665</v>
       </c>
     </row>
     <row r="12">
@@ -1417,30 +1403,30 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>179.0</v>
+        <v>175.0</v>
       </c>
       <c r="D16" t="n">
-        <v>-24.745288004314787</v>
+        <v>-32.287775356910714</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>175.0</v>
+        <v>179.0</v>
       </c>
       <c r="D17" t="n">
-        <v>-26.42695754611781</v>
+        <v>-30.740067365068665</v>
       </c>
     </row>
     <row r="18">
@@ -1507,7 +1493,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2078.1353025864646</v>
+        <v>2258.007880379244</v>
       </c>
     </row>
     <row r="3">
@@ -1521,7 +1507,7 @@
         <v>1756.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-15.5011707941024</v>
+        <v>-22.232335180997204</v>
       </c>
     </row>
     <row r="4">
@@ -1577,30 +1563,30 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>700.0</v>
+        <v>1056.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-32.63191293379463</v>
+        <v>-6.466225456871354</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>1056.0</v>
+        <v>700.0</v>
       </c>
       <c r="D12" t="n">
-        <v>1.6295713455898233</v>
+        <v>-37.99844490512305</v>
       </c>
     </row>
     <row r="13">
@@ -1635,30 +1621,30 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>700.0</v>
+        <v>1056.0</v>
       </c>
       <c r="D17" t="n">
-        <v>-32.63191293379463</v>
+        <v>-6.466225456871354</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>1056.0</v>
+        <v>700.0</v>
       </c>
       <c r="D18" t="n">
-        <v>1.6295713455898233</v>
+        <v>-37.99844490512305</v>
       </c>
     </row>
     <row r="19">
@@ -1716,7 +1702,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1026.5487639282537</v>
+        <v>1115.4014830789038</v>
       </c>
     </row>
     <row r="3">
@@ -1727,10 +1713,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>732.773680329143</v>
+        <v>1198.1066332506894</v>
       </c>
       <c r="D3" t="n">
-        <v>-28.617742665719376</v>
+        <v>7.414832365426832</v>
       </c>
     </row>
     <row r="4">
@@ -1752,7 +1738,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>732.7736803291428</v>
+        <v>1198.1066332506891</v>
       </c>
     </row>
     <row r="6">
@@ -1772,16 +1758,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>732.773680329143</v>
+        <v>1198.1066332506894</v>
       </c>
       <c r="D9" t="n">
-        <v>-28.61774266571938</v>
+        <v>7.414832365426845</v>
       </c>
     </row>
     <row r="10">
@@ -1791,13 +1777,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>198.91935977425555</v>
+        <v>211.93679608127758</v>
       </c>
     </row>
     <row r="12">
@@ -1807,13 +1793,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>533.8543205548874</v>
+        <v>986.1698371694118</v>
       </c>
     </row>
   </sheetData>
@@ -1855,7 +1841,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>3405.137363274208</v>
+        <v>3699.8683341153883</v>
       </c>
     </row>
     <row r="3">
@@ -1866,10 +1852,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>3911.66982401766</v>
+        <v>4060.0261172146</v>
       </c>
       <c r="D3" t="n">
-        <v>14.87553677589077</v>
+        <v>9.73434053796735</v>
       </c>
     </row>
     <row r="4">
@@ -1880,7 +1866,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>3911.66982401766</v>
+        <v>4060.0261172146</v>
       </c>
     </row>
     <row r="5">
@@ -1906,10 +1892,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>3911.66982401766</v>
+        <v>4060.0261172146</v>
       </c>
       <c r="D8" t="n">
-        <v>14.875536775890774</v>
+        <v>9.734340537967359</v>
       </c>
     </row>
     <row r="9">
@@ -2016,7 +2002,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>439.96965235026425</v>
+        <v>474.4893303917851</v>
       </c>
     </row>
     <row r="22">
@@ -2038,7 +2024,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>439.9696523502642</v>
+        <v>474.489330391785</v>
       </c>
     </row>
     <row r="24">
@@ -2059,7 +2045,7 @@
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>180.11772972929793</v>
+        <v>206.34916011947388</v>
       </c>
     </row>
     <row r="27">
@@ -2081,7 +2067,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>180.1177297292979</v>
+        <v>206.34916011947385</v>
       </c>
     </row>
     <row r="29">
@@ -2145,7 +2131,7 @@
         <v>6</v>
       </c>
       <c r="C36" t="n">
-        <v>420.79182490972346</v>
+        <v>444.73664720583577</v>
       </c>
     </row>
     <row r="37">
@@ -2167,7 +2153,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="n">
-        <v>420.7918249097234</v>
+        <v>444.7366472058357</v>
       </c>
     </row>
     <row r="39">
@@ -2188,7 +2174,7 @@
         <v>6</v>
       </c>
       <c r="C41" t="n">
-        <v>1437.1426639176925</v>
+        <v>1500.8030263868236</v>
       </c>
     </row>
     <row r="42">
@@ -2210,7 +2196,7 @@
         <v>6</v>
       </c>
       <c r="C43" t="n">
-        <v>1437.1426639176923</v>
+        <v>1500.8030263868234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on ACBalanceManager charts
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/WEIGHTS/Weights.xlsx
@@ -115,28 +115,28 @@
     <t>WEIGHT ESTIMATION METHODS COMPARISON</t>
   </si>
   <si>
+    <t>ROSKAM</t>
+  </si>
+  <si>
+    <t>RAYMER</t>
+  </si>
+  <si>
+    <t>NICOLAI_1984</t>
+  </si>
+  <si>
     <t>TORENBEEK_1976</t>
   </si>
   <si>
-    <t>RAYMER</t>
+    <t>TORENBEEK_2013</t>
+  </si>
+  <si>
+    <t>JENKINSON</t>
+  </si>
+  <si>
+    <t>SADRAEY</t>
   </si>
   <si>
     <t>KROO</t>
-  </si>
-  <si>
-    <t>SADRAEY</t>
-  </si>
-  <si>
-    <t>NICOLAI_1984</t>
-  </si>
-  <si>
-    <t>JENKINSON</t>
-  </si>
-  <si>
-    <t>TORENBEEK_2013</t>
-  </si>
-  <si>
-    <t>ROSKAM</t>
   </si>
   <si>
     <t>TORENBEEK_1982</t>
@@ -347,7 +347,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>27207.06814830184</v>
+        <v>27088.77555589343</v>
       </c>
     </row>
     <row r="6">
@@ -358,7 +358,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>26799.06814830184</v>
+        <v>26680.77555589343</v>
       </c>
     </row>
     <row r="7">
@@ -369,7 +369,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>24486.361333471657</v>
+        <v>24379.898000304085</v>
       </c>
     </row>
     <row r="8">
@@ -391,7 +391,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>5255.574895193706</v>
+        <v>5111.355631455008</v>
       </c>
     </row>
     <row r="10">
@@ -402,7 +402,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>21951.493253108136</v>
+        <v>21977.41992443842</v>
       </c>
     </row>
     <row r="11">
@@ -413,7 +413,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>21543.493253108136</v>
+        <v>21569.41992443842</v>
       </c>
     </row>
     <row r="12">
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>14607.493253108136</v>
+        <v>14633.419924438425</v>
       </c>
     </row>
     <row r="15">
@@ -457,7 +457,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>14377.949607608134</v>
+        <v>14403.876278938424</v>
       </c>
     </row>
     <row r="16">
@@ -501,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>13757.525607608139</v>
+        <v>13783.452278938428</v>
       </c>
     </row>
     <row r="20">
@@ -512,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>7941.499490393542</v>
+        <v>7966.897031846644</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2720.4914221436675</v>
+        <v>2708.6630703297674</v>
       </c>
     </row>
     <row r="3">
@@ -565,10 +565,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>3523.0</v>
+        <v>3534.75</v>
       </c>
       <c r="D3" t="n">
-        <v>29.498662312413344</v>
+        <v>30.497958152087918</v>
       </c>
     </row>
     <row r="4">
@@ -590,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>3522.9999999999995</v>
+        <v>3534.7499999999995</v>
       </c>
     </row>
     <row r="6">
@@ -611,10 +611,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>4094.0</v>
+        <v>4224.0</v>
       </c>
       <c r="D8" t="n">
-        <v>50.48751731678124</v>
+        <v>55.944090878964424</v>
       </c>
     </row>
     <row r="9">
@@ -625,10 +625,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>3151.0</v>
+        <v>3144.0</v>
       </c>
       <c r="D9" t="n">
-        <v>15.824662204488938</v>
+        <v>16.072022188320116</v>
       </c>
     </row>
     <row r="10">
@@ -639,10 +639,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>2378.0</v>
+        <v>3123.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-12.58932189074113</v>
+        <v>15.296731963779811</v>
       </c>
     </row>
     <row r="11">
@@ -653,10 +653,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2491.0</v>
+        <v>4094.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-8.435660567635056</v>
+        <v>51.14467520323872</v>
       </c>
     </row>
     <row r="12">
@@ -667,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>3127.0</v>
+        <v>3698.0</v>
       </c>
       <c r="D12" t="n">
-        <v>14.942468649138975</v>
+        <v>36.52491668333581</v>
       </c>
     </row>
     <row r="13">
@@ -684,7 +684,7 @@
         <v>5004.0</v>
       </c>
       <c r="D13" t="n">
-        <v>83.93735629046735</v>
+        <v>84.74058493331866</v>
       </c>
     </row>
     <row r="14">
@@ -695,10 +695,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>3698.0</v>
+        <v>2491.0</v>
       </c>
       <c r="D14" t="n">
-        <v>35.93132365350685</v>
+        <v>-8.035811936671307</v>
       </c>
     </row>
     <row r="15">
@@ -709,10 +709,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>4241.0</v>
+        <v>2500.0</v>
       </c>
       <c r="D15" t="n">
-        <v>55.890952843299765</v>
+        <v>-7.703544697582604</v>
       </c>
     </row>
   </sheetData>
@@ -754,7 +754,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2883.7209074722878</v>
+        <v>2871.182854549553</v>
       </c>
     </row>
     <row r="3">
@@ -765,10 +765,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>2303.75</v>
+        <v>2322.5</v>
       </c>
       <c r="D3" t="n">
-        <v>-20.11189453075952</v>
+        <v>-19.109993418919103</v>
       </c>
     </row>
     <row r="4">
@@ -790,7 +790,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>2303.7499999999995</v>
+        <v>2322.4999999999995</v>
       </c>
     </row>
     <row r="6">
@@ -805,30 +805,30 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>2283.0</v>
+        <v>2578.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-20.831450988051646</v>
+        <v>-10.21122197372375</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>2500.0</v>
+        <v>2121.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-13.306450928659272</v>
+        <v>-26.12800690700856</v>
       </c>
     </row>
     <row r="10">
@@ -842,21 +842,21 @@
         <v>2308.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-19.96451549733824</v>
+        <v>-19.61501175925307</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2124.0</v>
+        <v>2283.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-26.345160708988917</v>
+        <v>-20.48573303569097</v>
       </c>
     </row>
   </sheetData>
@@ -898,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>312.8565135465218</v>
+        <v>311.49625308792326</v>
       </c>
     </row>
     <row r="3">
@@ -912,7 +912,7 @@
         <v>237.5</v>
       </c>
       <c r="D3" t="n">
-        <v>-24.086605291443377</v>
+        <v>-23.755102141481295</v>
       </c>
     </row>
     <row r="4">
@@ -949,72 +949,72 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>276.0</v>
+        <v>124.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-11.780644465003677</v>
+        <v>-60.19213753913128</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>144.0</v>
+        <v>251.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-53.972510155654085</v>
+        <v>-19.42118163162866</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>303.0</v>
+        <v>144.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-3.1504901191888184</v>
+        <v>-53.77151456157181</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>124.0</v>
+        <v>276.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-60.36521707847991</v>
+        <v>-11.39540290967932</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>271.0</v>
+        <v>238.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-13.378821195710133</v>
+        <v>-23.594586567042313</v>
       </c>
     </row>
     <row r="13">
@@ -1028,21 +1028,21 @@
         <v>293.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-6.346843580601728</v>
+        <v>-5.93787337875377</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>238.0</v>
+        <v>271.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-23.926787618372735</v>
+        <v>-13.000558654069186</v>
       </c>
     </row>
     <row r="15">
@@ -1053,10 +1053,10 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>251.0</v>
+        <v>303.0</v>
       </c>
       <c r="D15" t="n">
-        <v>-19.771528118535954</v>
+        <v>-2.7275618899740355</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1098,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>312.8565135465218</v>
+        <v>311.49625308792326</v>
       </c>
     </row>
     <row r="3">
@@ -1109,10 +1109,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>325.1428571428571</v>
+        <v>324.8571428571428</v>
       </c>
       <c r="D3" t="n">
-        <v>3.9271496882254904</v>
+        <v>4.28926179264452</v>
       </c>
     </row>
     <row r="4">
@@ -1134,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>325.1428571428571</v>
+        <v>324.8571428571428</v>
       </c>
     </row>
     <row r="6">
@@ -1155,10 +1155,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>391.0</v>
+        <v>278.0</v>
       </c>
       <c r="D8" t="n">
-        <v>24.97742034124479</v>
+        <v>-10.753340611923372</v>
       </c>
     </row>
     <row r="9">
@@ -1169,38 +1169,38 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>89.0</v>
+        <v>88.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-71.55245419342509</v>
+        <v>-71.74925889873833</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>257.0</v>
+        <v>391.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-17.85371604168821</v>
+        <v>25.52317921128763</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>419.0</v>
+        <v>512.0</v>
       </c>
       <c r="D11" t="n">
-        <v>33.92721003320094</v>
+        <v>64.36794822552243</v>
       </c>
     </row>
     <row r="12">
@@ -1214,21 +1214,21 @@
         <v>330.0</v>
       </c>
       <c r="D12" t="n">
-        <v>5.479664226626039</v>
+        <v>5.940279129731248</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>512.0</v>
+        <v>419.0</v>
       </c>
       <c r="D13" t="n">
-        <v>63.65329722434101</v>
+        <v>34.51205137987089</v>
       </c>
     </row>
     <row r="14">
@@ -1239,10 +1239,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>278.0</v>
+        <v>256.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-11.141373772721094</v>
+        <v>-17.81602588723879</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>516.8933702072968</v>
+        <v>514.6459833626557</v>
       </c>
     </row>
     <row r="3">
@@ -1298,7 +1298,7 @@
         <v>354.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-31.513921360989688</v>
+        <v>-31.21485225882998</v>
       </c>
     </row>
     <row r="4">
@@ -1345,30 +1345,30 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>175.0</v>
+        <v>179.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-32.287775356910714</v>
+        <v>-30.43761895102015</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>179.0</v>
+        <v>175.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-30.740067365068665</v>
+        <v>-31.99208556663981</v>
       </c>
     </row>
     <row r="12">
@@ -1403,30 +1403,30 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>175.0</v>
+        <v>179.0</v>
       </c>
       <c r="D16" t="n">
-        <v>-32.287775356910714</v>
+        <v>-30.43761895102015</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>179.0</v>
+        <v>175.0</v>
       </c>
       <c r="D17" t="n">
-        <v>-30.740067365068665</v>
+        <v>-31.99208556663981</v>
       </c>
     </row>
     <row r="18">
@@ -1493,7 +1493,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2258.007880379244</v>
+        <v>2248.190348373707</v>
       </c>
     </row>
     <row r="3">
@@ -1507,7 +1507,7 @@
         <v>1756.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-22.232335180997204</v>
+        <v>-21.892734693472327</v>
       </c>
     </row>
     <row r="4">
@@ -1563,30 +1563,30 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>1056.0</v>
+        <v>700.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-6.466225456871354</v>
+        <v>-37.72769280800755</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>700.0</v>
+        <v>1056.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-37.99844490512305</v>
+        <v>-6.057776578937104</v>
       </c>
     </row>
     <row r="13">
@@ -1621,30 +1621,30 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>1056.0</v>
+        <v>700.0</v>
       </c>
       <c r="D17" t="n">
-        <v>-6.466225456871354</v>
+        <v>-37.72769280800755</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>700.0</v>
+        <v>1056.0</v>
       </c>
       <c r="D18" t="n">
-        <v>-37.99844490512305</v>
+        <v>-6.057776578937104</v>
       </c>
     </row>
     <row r="19">
@@ -1702,7 +1702,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1115.4014830789038</v>
+        <v>1110.5518588352047</v>
       </c>
     </row>
     <row r="3">
@@ -1713,10 +1713,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1198.1066332506894</v>
+        <v>1193.2898889895037</v>
       </c>
       <c r="D3" t="n">
-        <v>7.414832365426832</v>
+        <v>7.450172587264695</v>
       </c>
     </row>
     <row r="4">
@@ -1738,7 +1738,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>1198.1066332506891</v>
+        <v>1193.2898889895034</v>
       </c>
     </row>
     <row r="6">
@@ -1758,16 +1758,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>1198.1066332506894</v>
+        <v>1193.2898889895037</v>
       </c>
       <c r="D9" t="n">
-        <v>7.414832365426845</v>
+        <v>7.450172587264696</v>
       </c>
     </row>
     <row r="10">
@@ -1777,13 +1777,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>211.93679608127758</v>
+        <v>211.23048033263856</v>
       </c>
     </row>
     <row r="12">
@@ -1793,13 +1793,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>986.1698371694118</v>
+        <v>982.0594086568651</v>
       </c>
     </row>
   </sheetData>
@@ -1841,7 +1841,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>3699.8683341153883</v>
+        <v>3683.7817756484837</v>
       </c>
     </row>
     <row r="3">
@@ -1852,10 +1852,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>4060.0261172146</v>
+        <v>4060.55524709179</v>
       </c>
       <c r="D3" t="n">
-        <v>9.73434053796735</v>
+        <v>10.227898784177562</v>
       </c>
     </row>
     <row r="4">
@@ -1866,7 +1866,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>4060.0261172146</v>
+        <v>4060.55524709179</v>
       </c>
     </row>
     <row r="5">
@@ -1892,10 +1892,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>4060.0261172146</v>
+        <v>4060.55524709179</v>
       </c>
       <c r="D8" t="n">
-        <v>9.734340537967359</v>
+        <v>10.227898784177574</v>
       </c>
     </row>
     <row r="9">
@@ -2002,7 +2002,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>474.4893303917851</v>
+        <v>474.9841522184727</v>
       </c>
     </row>
     <row r="22">
@@ -2024,7 +2024,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>474.489330391785</v>
+        <v>474.9841522184726</v>
       </c>
     </row>
     <row r="24">
@@ -2045,7 +2045,7 @@
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>206.34916011947388</v>
+        <v>206.736663273393</v>
       </c>
     </row>
     <row r="27">
@@ -2067,7 +2067,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>206.34916011947385</v>
+        <v>206.73666327339296</v>
       </c>
     </row>
     <row r="29">
@@ -2131,7 +2131,7 @@
         <v>6</v>
       </c>
       <c r="C36" t="n">
-        <v>444.73664720583577</v>
+        <v>443.4465411358582</v>
       </c>
     </row>
     <row r="37">
@@ -2153,7 +2153,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="n">
-        <v>444.7366472058357</v>
+        <v>443.4465411358581</v>
       </c>
     </row>
     <row r="39">
@@ -2174,7 +2174,7 @@
         <v>6</v>
       </c>
       <c r="C41" t="n">
-        <v>1500.8030263868236</v>
+        <v>1501.739937353384</v>
       </c>
     </row>
     <row r="42">
@@ -2196,7 +2196,7 @@
         <v>6</v>
       </c>
       <c r="C43" t="n">
-        <v>1500.8030263868234</v>
+        <v>1501.739937353384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>